<commit_message>
Major app.py and html Update
</commit_message>
<xml_diff>
--- a/app/static/test.xlsx
+++ b/app/static/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zach Vohra\Documents\GITHUB\seatingPlan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zach Vohra\Documents\GITHUB\Cinema-Booking\app\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E8428F-4E8F-4AD1-9EE6-FACE8FBE1B4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B404ED5-9104-4439-9EF1-7576A971F760}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,15 +32,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>🎬 SCREEN 🎬</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
   <si>
     <t>BLOCK A</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
   <si>
     <t>Adult</t>
@@ -55,25 +61,16 @@
     <t>BLOCK B</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>P</t>
   </si>
   <si>
     <t>KEY</t>
   </si>
   <si>
     <t>Basket</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
   <si>
     <t>💲 INCOME 💲</t>
@@ -2840,8 +2837,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="AA29" sqref="AA29"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AW25" sqref="AW25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2850,7 +2847,7 @@
     <col min="27" max="27" width="10" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2876,7 +2873,7 @@
       <c r="V1" s="11"/>
       <c r="W1" s="12"/>
     </row>
-    <row r="2" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="13"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -2900,12 +2897,7 @@
       <c r="V2" s="14"/>
       <c r="W2" s="15"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -2927,10 +2919,10 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="AA4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -2952,14 +2944,14 @@
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="AA5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AB5">
         <f>COUNTIF(B4:K23,"A")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -2981,14 +2973,14 @@
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="AA6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AB6">
         <f>COUNTIF(B4:K23,"P")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -3010,14 +3002,14 @@
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="AA7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AB7">
         <f>COUNTIF(B4:K23,"C")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -3039,7 +3031,7 @@
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -3061,7 +3053,7 @@
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -3083,10 +3075,10 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="AA10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -3108,14 +3100,14 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="AA11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AB11">
         <f>COUNTIF(N4:W23,"A")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -3137,14 +3129,14 @@
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="AA12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AB12">
         <f>COUNTIF(N4:W23,"P")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -3166,14 +3158,14 @@
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="AA13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AB13">
         <f>COUNTIF(N4:W23,"C")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -3195,7 +3187,7 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -3217,7 +3209,7 @@
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -3264,7 +3256,7 @@
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="AA17" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AB17">
         <f>AB11+AB5</f>
@@ -3293,7 +3285,7 @@
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="AA18" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AB18">
         <f>AB6+AB12</f>
@@ -3322,7 +3314,7 @@
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="AA19" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AB19">
         <f>AB7+AB13</f>
@@ -3395,7 +3387,7 @@
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="AA22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.25">
@@ -3420,23 +3412,23 @@
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="AA23" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AB23" s="2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AA24" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AB24" s="3" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="2:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -3448,7 +3440,7 @@
       <c r="J25" s="17"/>
       <c r="K25" s="18"/>
       <c r="N25" s="16" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O25" s="17"/>
       <c r="P25" s="17"/>
@@ -3460,18 +3452,18 @@
       <c r="V25" s="17"/>
       <c r="W25" s="18"/>
       <c r="AA25" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AB25" s="4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.25">
       <c r="AA26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AB26" s="8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -4605,7 +4597,7 @@
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -4613,21 +4605,21 @@
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6" s="6">
         <v>10</v>
@@ -4643,7 +4635,7 @@
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C7" s="6">
         <v>7</v>
@@ -4659,7 +4651,7 @@
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" s="6">
         <v>5</v>
@@ -4678,7 +4670,7 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="7">
         <f>SUM(E6:E8)</f>
@@ -4687,13 +4679,13 @@
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
       <c r="E13" s="21"/>
       <c r="G13" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
@@ -4701,7 +4693,7 @@
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E15" s="7">
         <v>500</v>
@@ -4719,7 +4711,7 @@
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" s="7">
         <v>80</v>
@@ -4727,7 +4719,7 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" s="7">
         <v>65</v>
@@ -4735,7 +4727,7 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="7">
         <v>125</v>
@@ -4743,7 +4735,7 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E19" s="7">
         <v>35</v>
@@ -4751,7 +4743,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E20" s="7">
         <v>70</v>
@@ -4759,7 +4751,7 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" s="7">
         <v>0</v>
@@ -4767,7 +4759,7 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E23" s="7">
         <f>SUM(E15:E21)</f>

</xml_diff>